<commit_message>
added SchemaSchema to template document
</commit_message>
<xml_diff>
--- a/dmcar_serialisation_template.xlsx
+++ b/dmcar_serialisation_template.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DMCAR" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Mapping" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Requirement" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Schema" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Requirement" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="81">
   <si>
     <t xml:space="preserve">Namespace</t>
   </si>
@@ -208,6 +209,45 @@
   </si>
   <si>
     <t xml:space="preserve">http://www.tkltd.org/ontologies/datamodel#Relationship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SchemaLabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SchemaDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ValueConstraints</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MetaDataDomain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SchemaSchema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{“String”, “Integer”, “Date”, “DateTime”, “Float”, “Boolean”, “Image”, “Schema", “Collection"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{“Yes”, “No”}</t>
   </si>
   <si>
     <t xml:space="preserve">Project</t>
@@ -545,11 +585,11 @@
   </sheetPr>
   <dimension ref="A1:AN1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.91"/>
@@ -732,7 +772,7 @@
       <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="22.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="33.39"/>
@@ -1739,13 +1779,737 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:R19"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="22.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="6.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="19.63"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q8" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q9" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="P10" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q10" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="P11" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q11" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="P12" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q12" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="P13" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q13" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="P14" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q14" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="P15" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q15" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="L16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="P16" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q16" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="L17" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="P17" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q17" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="R17" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="P18" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q18" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="R18" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I19" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="M19" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="O19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="P19" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q19" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
@@ -1758,22 +2522,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added visualisation code, colourschemes and some sample data.
</commit_message>
<xml_diff>
--- a/dmcar_serialisation_template.xlsx
+++ b/dmcar_serialisation_template.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="80">
   <si>
     <t xml:space="preserve">Namespace</t>
   </si>
@@ -226,9 +226,6 @@
     <t xml:space="preserve">Meta</t>
   </si>
   <si>
-    <t xml:space="preserve">MetaDataDomain</t>
-  </si>
-  <si>
     <t xml:space="preserve">SchemaSchema</t>
   </si>
   <si>
@@ -244,7 +241,7 @@
     <t xml:space="preserve">Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">{“String”, “Integer”, “Date”, “DateTime”, “Float”, “Boolean”, “Image”, “Schema", “Collection"}</t>
+    <t xml:space="preserve">{“String”, “Integer”, “Date”, “DateTime”, “Float”, “Boolean”, “Image”, “Collection" } or &lt;Schema&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">{“Yes”, “No”}</t>
@@ -1779,10 +1776,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1791,20 +1788,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="22.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="22.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="6.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="19.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="19.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1820,46 +1813,34 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>64</v>
       </c>
+      <c r="H1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="L1" s="6" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="R1" s="6" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1876,26 +1857,20 @@
       <c r="F2" s="0" t="s">
         <v>67</v>
       </c>
+      <c r="H2" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="I2" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="J2" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>0</v>
-      </c>
       <c r="M2" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="P2" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1911,26 +1886,20 @@
       <c r="F3" s="0" t="s">
         <v>67</v>
       </c>
+      <c r="H3" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="I3" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L3" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="J3" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>1</v>
-      </c>
       <c r="M3" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="O3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="P3" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q3" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1946,26 +1915,20 @@
       <c r="F4" s="0" t="s">
         <v>67</v>
       </c>
+      <c r="H4" s="0" t="s">
+        <v>2</v>
+      </c>
       <c r="I4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L4" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="J4" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>2</v>
-      </c>
       <c r="M4" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="O4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="P4" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q4" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1981,26 +1944,20 @@
       <c r="F5" s="0" t="s">
         <v>67</v>
       </c>
+      <c r="H5" s="0" t="s">
+        <v>3</v>
+      </c>
       <c r="I5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L5" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="J5" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>3</v>
-      </c>
       <c r="M5" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="O5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="P5" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q5" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2016,26 +1973,20 @@
       <c r="F6" s="0" t="s">
         <v>67</v>
       </c>
+      <c r="H6" s="0" t="s">
+        <v>62</v>
+      </c>
       <c r="I6" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="L6" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="J6" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>4</v>
-      </c>
       <c r="M6" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="O6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="P6" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="Q6" s="0" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2051,26 +2002,20 @@
       <c r="F7" s="0" t="s">
         <v>67</v>
       </c>
+      <c r="H7" s="0" t="s">
+        <v>63</v>
+      </c>
       <c r="I7" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="L7" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="J7" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>5</v>
-      </c>
       <c r="M7" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="O7" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="P7" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q7" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2086,26 +2031,20 @@
       <c r="F8" s="0" t="s">
         <v>67</v>
       </c>
+      <c r="H8" s="0" t="s">
+        <v>64</v>
+      </c>
       <c r="I8" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="L8" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="J8" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="L8" s="0" t="s">
-        <v>6</v>
-      </c>
       <c r="M8" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="O8" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="P8" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q8" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2121,26 +2060,20 @@
       <c r="F9" s="0" t="s">
         <v>67</v>
       </c>
+      <c r="H9" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="I9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="L9" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="J9" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="L9" s="0" t="s">
-        <v>7</v>
-      </c>
       <c r="M9" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="O9" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="P9" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="Q9" s="0" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2156,25 +2089,19 @@
       <c r="F10" s="0" t="s">
         <v>67</v>
       </c>
+      <c r="H10" s="0" t="s">
+        <v>22</v>
+      </c>
       <c r="I10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="L10" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="J10" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="L10" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="M10" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="O10" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="P10" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q10" s="0" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2191,26 +2118,20 @@
       <c r="F11" s="0" t="s">
         <v>67</v>
       </c>
+      <c r="H11" s="0" t="s">
+        <v>23</v>
+      </c>
       <c r="I11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L11" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="J11" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="L11" s="0" t="s">
-        <v>63</v>
-      </c>
       <c r="M11" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="O11" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="P11" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q11" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2226,26 +2147,20 @@
       <c r="F12" s="0" t="s">
         <v>67</v>
       </c>
+      <c r="H12" s="0" t="s">
+        <v>24</v>
+      </c>
       <c r="I12" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>68</v>
+        <v>24</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>11</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="O12" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="P12" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q12" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2261,26 +2176,23 @@
       <c r="F13" s="0" t="s">
         <v>67</v>
       </c>
+      <c r="H13" s="0" t="s">
+        <v>25</v>
+      </c>
       <c r="I13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="L13" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="J13" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="L13" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="M13" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="O13" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="P13" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q13" s="0" t="s">
         <v>70</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2296,195 +2208,46 @@
       <c r="F14" s="0" t="s">
         <v>67</v>
       </c>
+      <c r="H14" s="0" t="s">
+        <v>26</v>
+      </c>
       <c r="I14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="L14" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="J14" s="0" t="s">
+      <c r="M14" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="N14" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="L15" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="L14" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="M14" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="O14" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="P14" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q14" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="J15" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="L15" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="M15" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="O15" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="P15" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q15" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="J16" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="L16" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="M16" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="O16" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="P16" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q16" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="L17" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="M17" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="O17" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="P17" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q17" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="R17" s="0" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="L18" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="M18" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="O18" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="P18" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q18" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="R18" s="0" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I19" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="L19" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="M19" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="O19" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="P19" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q19" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2522,22 +2285,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor refactor loader content to graphloader.py, ontology tweaks
</commit_message>
<xml_diff>
--- a/dmcar_serialisation_template.xlsx
+++ b/dmcar_serialisation_template.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="80">
   <si>
     <t xml:space="preserve">Namespace</t>
   </si>
@@ -582,11 +582,11 @@
   </sheetPr>
   <dimension ref="A1:AN1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.91"/>
@@ -765,11 +765,11 @@
   </sheetPr>
   <dimension ref="A1:M158"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="22.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="33.39"/>
@@ -1776,23 +1776,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.43"/>
@@ -1945,19 +1945,19 @@
         <v>67</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L5" s="0" t="s">
         <v>68</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1974,19 +1974,19 @@
         <v>67</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K6" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L6" s="0" t="s">
         <v>68</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2003,13 +2003,13 @@
         <v>67</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L7" s="0" t="s">
         <v>68</v>
@@ -2032,19 +2032,19 @@
         <v>67</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="K8" s="0" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L8" s="0" t="s">
         <v>68</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2061,19 +2061,19 @@
         <v>67</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K9" s="0" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L9" s="0" t="s">
         <v>68</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2090,13 +2090,13 @@
         <v>67</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K10" s="0" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L10" s="0" t="s">
         <v>68</v>
@@ -2119,16 +2119,16 @@
         <v>67</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K11" s="0" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="M11" s="0" t="s">
         <v>70</v>
@@ -2148,20 +2148,23 @@
         <v>67</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K12" s="0" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="M12" s="0" t="s">
         <v>70</v>
       </c>
+      <c r="N12" s="0" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -2177,13 +2180,13 @@
         <v>67</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K13" s="0" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L13" s="0" t="s">
         <v>68</v>
@@ -2192,16 +2195,10 @@
         <v>70</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>66</v>
-      </c>
       <c r="E14" s="0" t="s">
         <v>67</v>
       </c>
@@ -2209,44 +2206,18 @@
         <v>67</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="K14" s="0" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L14" s="0" t="s">
         <v>68</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="N14" s="0" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E15" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="K15" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="L15" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="M15" s="0" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2272,7 +2243,7 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>

</xml_diff>

<commit_message>
added pipenv python environment
</commit_message>
<xml_diff>
--- a/dmcar_serialisation_template.xlsx
+++ b/dmcar_serialisation_template.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="80">
   <si>
     <t xml:space="preserve">Namespace</t>
   </si>
@@ -586,7 +586,7 @@
       <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.91"/>
@@ -769,7 +769,7 @@
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.5625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="22.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="33.39"/>
@@ -1778,21 +1778,21 @@
   </sheetPr>
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.43"/>
@@ -2199,6 +2199,12 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>66</v>
+      </c>
       <c r="E14" s="0" t="s">
         <v>67</v>
       </c>
@@ -2243,7 +2249,7 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>

</xml_diff>